<commit_message>
more git commands added
</commit_message>
<xml_diff>
--- a/How-To.xlsx
+++ b/How-To.xlsx
@@ -9,25 +9,27 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19575" windowHeight="6285" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19260" windowHeight="6285"/>
   </bookViews>
   <sheets>
     <sheet name="MISC" sheetId="1" r:id="rId1"/>
     <sheet name="git" sheetId="2" r:id="rId2"/>
-    <sheet name="gdb" sheetId="3" r:id="rId3"/>
-    <sheet name="mysql" sheetId="4" r:id="rId4"/>
-    <sheet name="ubuntu" sheetId="5" r:id="rId5"/>
-    <sheet name="android" sheetId="6" r:id="rId6"/>
-    <sheet name="adb-fastboot" sheetId="7" r:id="rId7"/>
-    <sheet name="kernel-dbg" sheetId="8" r:id="rId8"/>
-    <sheet name="make kernel" sheetId="9" r:id="rId9"/>
+    <sheet name="how git works" sheetId="11" r:id="rId3"/>
+    <sheet name="gdb" sheetId="3" r:id="rId4"/>
+    <sheet name="mysql" sheetId="4" r:id="rId5"/>
+    <sheet name="ubuntu" sheetId="5" r:id="rId6"/>
+    <sheet name="android" sheetId="6" r:id="rId7"/>
+    <sheet name="adb-fastboot" sheetId="7" r:id="rId8"/>
+    <sheet name="kernel-dbg" sheetId="8" r:id="rId9"/>
+    <sheet name="make kernel" sheetId="9" r:id="rId10"/>
+    <sheet name="yocto" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="244">
   <si>
     <t>dump include info junk.i</t>
   </si>
@@ -558,18 +560,264 @@
   </si>
   <si>
     <t>verbose</t>
+  </si>
+  <si>
+    <t>git checkout -b LNX.LE.6.0 origin/LNX.LE.6.0</t>
+  </si>
+  <si>
+    <t>remote/origin/LNX.LE.6.0 (git branch -r)</t>
+  </si>
+  <si>
+    <t>git archive HEAD(HASH) --format=zip &gt; file.zip</t>
+  </si>
+  <si>
+    <t>goldfish cross compile</t>
+  </si>
+  <si>
+    <t>export PATH=/prebuilt/linux-x86/toolchain/arm-eabi-4.4.3/bin/:$PATH</t>
+  </si>
+  <si>
+    <t>make ARCH=arm goldfish_armv7_defconfig</t>
+  </si>
+  <si>
+    <r>
+      <t>CROSS_COMPILE=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/prebuilt/linux-x86/toolchain/arm-eabi-4.4.3/bin/arm-eabi- ARCH=arm make</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>export ANDROID_PRODUCT_OUT=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/out/target/product/generic/</t>
+    </r>
+  </si>
+  <si>
+    <t>git rev-parse HEAD/ --verify HEAD</t>
+  </si>
+  <si>
+    <t>show current commit</t>
+  </si>
+  <si>
+    <t>view current commit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git show || git log -1 | git status || </t>
+  </si>
+  <si>
+    <t>git checkout v1.2</t>
+  </si>
+  <si>
+    <t>checkout local tag</t>
+  </si>
+  <si>
+    <t>git config --global diff.tool=vimdiff</t>
+  </si>
+  <si>
+    <t>git difftool</t>
+  </si>
+  <si>
+    <t>config tool</t>
+  </si>
+  <si>
+    <t>show tools</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Descriptions</t>
+  </si>
+  <si>
+    <t>lots of debug info</t>
+  </si>
+  <si>
+    <t>bibake -DDD</t>
+  </si>
+  <si>
+    <t>bitbake -s</t>
+  </si>
+  <si>
+    <t>recipe version</t>
+  </si>
+  <si>
+    <t>bitbake -c</t>
+  </si>
+  <si>
+    <t>execute task for the image/recipe being built</t>
+  </si>
+  <si>
+    <t>option -g</t>
+  </si>
+  <si>
+    <t>output dependency tree</t>
+  </si>
+  <si>
+    <t>git tag -d tagname</t>
+  </si>
+  <si>
+    <t>delete tag</t>
+  </si>
+  <si>
+    <t>git diff --name-only SHA1 SHA2</t>
+  </si>
+  <si>
+    <t>git log --pretty=oneline</t>
+  </si>
+  <si>
+    <t>git log --pretty=format:"%h/H -- %cd %cn : %s"</t>
+  </si>
+  <si>
+    <t>%h abbreviated hash</t>
+  </si>
+  <si>
+    <t>%H long hash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%cn commit name </t>
+  </si>
+  <si>
+    <t>%s subject</t>
+  </si>
+  <si>
+    <t>%cd commit date</t>
+  </si>
+  <si>
+    <t>%an author name</t>
+  </si>
+  <si>
+    <t>git log -p -2</t>
+  </si>
+  <si>
+    <t>option -p show diff introduced in each commit</t>
+  </si>
+  <si>
+    <t>git show hash:filename &gt; file</t>
+  </si>
+  <si>
+    <t>cat file | git hash-object --stdin</t>
+  </si>
+  <si>
+    <t>cal sha and print out to stdin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cat file | shasum </t>
+  </si>
+  <si>
+    <t>printf "blob 0\0" | shasum</t>
+  </si>
+  <si>
+    <t>"blob size\0"</t>
+  </si>
+  <si>
+    <t>git cat-file -t SHA</t>
+  </si>
+  <si>
+    <t>option -t only show type</t>
+  </si>
+  <si>
+    <t>git cat-file -p SHA</t>
+  </si>
+  <si>
+    <t>pretty-print the contents of obj based on type</t>
+  </si>
+  <si>
+    <t>git cat-file -s SHA</t>
+  </si>
+  <si>
+    <t>object/file size</t>
+  </si>
+  <si>
+    <t>git config --global core.editor "vim"</t>
+  </si>
+  <si>
+    <t>git cat-file tag tag_name</t>
+  </si>
+  <si>
+    <t>dict A</t>
+  </si>
+  <si>
+    <t>README</t>
+  </si>
+  <si>
+    <t>test.rb</t>
+  </si>
+  <si>
+    <t>LICENSE</t>
+  </si>
+  <si>
+    <t>tree content</t>
+  </si>
+  <si>
+    <t>commit content (initial)</t>
+  </si>
+  <si>
+    <t>new commit (B)</t>
+  </si>
+  <si>
+    <t>commit B content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">made change on testing and commit </t>
+  </si>
+  <si>
+    <t>the parent of the master branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the content of the master commit (HEAD) </t>
+  </si>
+  <si>
+    <t>the contents of the testing commit (HEAd)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -608,6 +856,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -635,44 +889,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,7 +967,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>130507</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -751,8 +1016,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>285750</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -805,14 +1070,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>516046</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:colOff>382696</xdr:colOff>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>47624</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>514349</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>81319</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -843,8 +1108,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8802796" y="2771775"/>
-          <a:ext cx="3732103" cy="3405544"/>
+          <a:off x="10945921" y="3152775"/>
+          <a:ext cx="3732103" cy="3215044"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -859,6 +1124,1149 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>509975</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EB6BEB8-D94C-4EE8-9F25-B5B971ED4017}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7000875" y="4333875"/>
+          <a:ext cx="4072325" cy="2628900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>258743</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="enter image description here">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3789D51-D76A-4BC5-A90F-E4708BE184E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6962775" y="7048500"/>
+          <a:ext cx="3259118" cy="2047875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>940049</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="A commit and its tree.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C94743AD-2ED0-4E4C-9625-D0A48B1F4FDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2159249" y="400050"/>
+          <a:ext cx="6175125" cy="3419475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>55831</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB6DBC18-CA87-4C19-8AED-9E7D10D106AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="4000500"/>
+          <a:ext cx="6829425" cy="817831"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3980952</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38024</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00E21EDD-596D-4D33-BA11-CE45733F02FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="4953000"/>
+          <a:ext cx="3980952" cy="609524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>294396</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>190408</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57DFBEC4-8BB0-4877-B7BF-254E3EB453BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5934075"/>
+          <a:ext cx="7028571" cy="733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>18206</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>190405</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B444F08-6E88-4EB9-8E0D-6FD8575E13D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="7048500"/>
+          <a:ext cx="6752381" cy="761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>226263</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="Commits and their parents.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A45C10C-7990-473A-8A67-AB4AA78485F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9560763" y="342900"/>
+          <a:ext cx="6469811" cy="2143125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3523809</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>76119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F3A1BBA-F862-471A-850E-7879FE51214E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="8191500"/>
+          <a:ext cx="3523809" cy="647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>284873</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>142719</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{777BC03C-87DC-4221-939B-7D1E871B4073}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="9182100"/>
+          <a:ext cx="7019048" cy="1247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>391704</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="Two branches pointing into the same series of commits.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A2DB9AE-154A-4487-85DA-8FAF0C670CA4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8345079" y="4229101"/>
+          <a:ext cx="3913595" cy="1619250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>179595</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>124695</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="HEAD pointing to a branch.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B996E53E-62C4-461A-BD3A-34CAC25035F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8753475" y="6275595"/>
+          <a:ext cx="3495675" cy="2040600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>170714</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>9262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{288FE48E-4864-4AD9-AAEF-F5917AD45845}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="10668000"/>
+          <a:ext cx="5885714" cy="2104762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>332492</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>114167</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC231829-16F8-4A12-8C63-E44A6F099718}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="13144500"/>
+          <a:ext cx="7066667" cy="1066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>536765</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>17510</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18" descr="The HEAD branch moves forward when a commit is made.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B19B9A6E-6198-49DC-8995-D7F731C2D3C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7880540" y="8743950"/>
+          <a:ext cx="4357545" cy="1819275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>324877</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19" descr="HEAD moves when you checkout.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F9672CF-BB28-45F2-A90E-6C7B1456FF1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7953375" y="11277600"/>
+          <a:ext cx="5201677" cy="2171700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>169068</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21" descr="Divergent history.">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF50B07D-DC40-4728-BD09-9B399041A513}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7953375" y="14287500"/>
+          <a:ext cx="5655468" cy="3619500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>370894</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>133262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7317A33F-148E-49C9-9F9F-484CB468F7FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="14668500"/>
+          <a:ext cx="4647619" cy="704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>418513</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>142786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7055723-47C6-4F48-A3D3-C422F0EBCD96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="17716500"/>
+          <a:ext cx="4695238" cy="714286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3752850</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EC847EA-4F2E-499A-BD09-53DFF6D910BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="600075" y="15592425"/>
+          <a:ext cx="3762375" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>105561</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43F8A1A9-7074-490E-9928-091CE66E0AEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="600075" y="16592550"/>
+          <a:ext cx="5305425" cy="848511"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>237380</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>9412</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="Picture 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F6B7E5C-0342-4814-99E7-B1A8B4FF2D2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="600075" y="18916650"/>
+          <a:ext cx="5961905" cy="904762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1155,8 +2563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C47"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1358,12 +2766,229 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:C25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="88" style="5" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3">
+      <c r="B3" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="30">
+      <c r="B10" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="B14" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="30">
+      <c r="B16" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" s="16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" s="15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="4" width="44.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:4">
+      <c r="C3" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4">
+      <c r="C4" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4">
+      <c r="C5" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4">
+      <c r="C6" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4">
+      <c r="C7" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F55"/>
+  <dimension ref="B3:F90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1372,6 +2997,11 @@
     <col min="3" max="3" width="36" style="5" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
+    </row>
     <row r="4" spans="2:3">
       <c r="B4" t="s">
         <v>91</v>
@@ -1402,237 +3032,404 @@
     </row>
     <row r="9" spans="2:3">
       <c r="B9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="C10" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="C11" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="C12" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="C13" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3">
+      <c r="C14" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="30">
+      <c r="B15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="B16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
-      <c r="B10" t="s">
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>205</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
-      <c r="B11" t="s">
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
-      <c r="B13" t="s">
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="2:3">
-      <c r="B14" t="s">
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
-      <c r="C15" s="5" t="s">
+    <row r="25" spans="2:3">
+      <c r="C25" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
-      <c r="C16" s="5" t="s">
+    <row r="26" spans="2:3">
+      <c r="C26" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
-      <c r="B18" t="s">
+    <row r="28" spans="2:3">
+      <c r="B28" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
-      <c r="B19" t="s">
+    <row r="29" spans="2:3">
+      <c r="B29" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
-      <c r="B21" t="s">
+    <row r="31" spans="2:3">
+      <c r="B31" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
-      <c r="B22" t="s">
+    <row r="32" spans="2:3">
+      <c r="B32" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
-      <c r="C23" s="5" t="s">
+    <row r="33" spans="2:6">
+      <c r="C33" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
-      <c r="B24" t="s">
+    <row r="34" spans="2:6">
+      <c r="B34" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
-      <c r="B26" t="s">
+    <row r="36" spans="2:6">
+      <c r="B36" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
-      <c r="B27" t="s">
+    <row r="37" spans="2:6">
+      <c r="B37" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
-      <c r="B29" t="s">
+    <row r="39" spans="2:6">
+      <c r="B39" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="30">
-      <c r="B30" t="s">
+    <row r="40" spans="2:6" ht="30">
+      <c r="B40" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
-      <c r="B32" t="s">
+    <row r="42" spans="2:6">
+      <c r="B42" t="s">
         <v>111</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C42" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D32">
+      <c r="D42">
         <v>11520</v>
       </c>
-      <c r="E32">
+      <c r="E42">
         <v>2</v>
       </c>
-      <c r="F32">
-        <f>(D32*E32)</f>
+      <c r="F42">
+        <f>(D42*E42)</f>
         <v>23040</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
-      <c r="B34" t="s">
+    <row r="43" spans="2:6">
+      <c r="B43" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="2:3">
-      <c r="B35" t="s">
+    <row r="47" spans="2:6">
+      <c r="B47" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
-      <c r="B36" t="s">
+    <row r="48" spans="2:6">
+      <c r="B48" t="s">
         <v>114</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3">
-      <c r="B38" t="s">
-        <v>117</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3">
-      <c r="B40" t="s">
-        <v>119</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3">
-      <c r="B42" t="s">
-        <v>121</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3">
-      <c r="B44" t="s">
-        <v>133</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3">
-      <c r="B45" t="s">
-        <v>135</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3">
-      <c r="B47" t="s">
-        <v>137</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3">
-      <c r="B48" t="s">
-        <v>138</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="50" spans="2:3">
       <c r="B50" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" ht="30">
-      <c r="B51" t="s">
-        <v>142</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3">
-      <c r="B53" t="s">
-        <v>172</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>173</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3">
+      <c r="B52" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="2:3">
       <c r="B54" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3">
+      <c r="B56" t="s">
+        <v>133</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3">
+      <c r="B57" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3">
+      <c r="B59" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3">
+      <c r="B60" t="s">
+        <v>138</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3">
+      <c r="B62" t="s">
+        <v>140</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" ht="30">
+      <c r="B63" t="s">
+        <v>142</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="B65" t="s">
+        <v>172</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3">
+      <c r="B66" t="s">
         <v>82</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C66" s="5" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="55" spans="2:3">
-      <c r="B55" t="s">
+    <row r="67" spans="2:3">
+      <c r="B67" t="s">
         <v>175</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C67" s="5" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="30">
+      <c r="B69" t="s">
+        <v>177</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3">
+      <c r="B71" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3">
+      <c r="B73" t="s">
+        <v>185</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3">
+      <c r="B74" t="s">
+        <v>188</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3">
+      <c r="B76" t="s">
+        <v>191</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3">
+      <c r="B77" t="s">
+        <v>192</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3">
+      <c r="B79" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3">
+      <c r="B82" t="s">
+        <v>219</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" t="s">
+        <v>222</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3">
+      <c r="B86" t="s">
+        <v>224</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" ht="30">
+      <c r="B87" t="s">
+        <v>226</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3">
+      <c r="B88" t="s">
+        <v>228</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3">
+      <c r="B90" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -1643,6 +3440,89 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:D99"/>
+  <sheetViews>
+    <sheetView topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97:H99"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="64.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="C5" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="C6" s="5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="C22" s="18"/>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" s="19" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2">
+      <c r="B43" s="19" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2">
+      <c r="B48" s="19" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2">
+      <c r="B69" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2">
+      <c r="B87" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2">
+      <c r="B93" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2">
+      <c r="B99" t="s">
+        <v>242</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C12"/>
   <sheetViews>
@@ -1734,7 +3614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:B9"/>
   <sheetViews>
@@ -1772,7 +3652,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C12"/>
   <sheetViews>
@@ -1836,12 +3716,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1901,7 +3781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:D12"/>
   <sheetViews>
@@ -1957,7 +3837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:D9"/>
   <sheetViews>
@@ -2014,136 +3894,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:C17"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="60.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:3">
-      <c r="B3" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="30">
-      <c r="B10" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3">
-      <c r="B11" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3">
-      <c r="B13" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3">
-      <c r="B14" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="C14" s="14"/>
-    </row>
-    <row r="15" spans="2:3">
-      <c r="B15" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="30">
-      <c r="B16" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>